<commit_message>
[add] Class Readxl & Writexl & etc
1. checking Readxl and Writexl class
2. make Demo.py to test both class
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,57 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>1.0</t>
+    <t>data length</t>
   </si>
   <si>
-    <t>2.0</t>
+    <t>data list</t>
   </si>
   <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -396,81 +354,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>